<commit_message>
extend some feature: text bold / align/ color, but not complete
</commit_message>
<xml_diff>
--- a/packages/wasm/src/snapshots/imexport_wasm__tests__tests__export_data_should_be_correct.snap.xlsx
+++ b/packages/wasm/src/snapshots/imexport_wasm__tests__tests__export_data_should_be_correct.snap.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+  <si>
+    <t>Tom and Jerry</t>
+  </si>
   <si>
     <t>Name</t>
   </si>
@@ -38,7 +41,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -46,13 +49,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -67,8 +92,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -363,46 +393,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="30" customHeight="1"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" ht="50" customHeight="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:3" ht="30" customHeight="1">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
+    <row r="3" spans="1:3" ht="30" customHeight="1">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
+      <c r="C3" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+    <row r="4" spans="1:3" ht="30" customHeight="1">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
         <v>5</v>
-      </c>
-      <c r="B3">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add date format export support
</commit_message>
<xml_diff>
--- a/packages/wasm/src/snapshots/imexport_wasm__tests__tests__export_data_should_be_correct.snap.xlsx
+++ b/packages/wasm/src/snapshots/imexport_wasm__tests__tests__export_data_should_be_correct.snap.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Tom and Jerry</t>
   </si>
@@ -43,9 +43,6 @@
     <t>Tom</t>
   </si>
   <si>
-    <t>2021-01-01</t>
-  </si>
-  <si>
     <t>Love</t>
   </si>
   <si>
@@ -53,9 +50,6 @@
   </si>
   <si>
     <t>Jerry</t>
-  </si>
-  <si>
-    <t>2022-01-01</t>
   </si>
   <si>
     <t>Hate</t>
@@ -68,6 +62,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-MM-dd HH:mm"/>
+  </numFmts>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -118,7 +115,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -126,6 +123,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,31 +480,31 @@
       <c r="B5">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3">
+        <v>44197.35555555556</v>
+      </c>
+      <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" customHeight="1">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3">
+        <v>44562</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
         <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -518,23 +516,6 @@
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E2:E4"/>
   </mergeCells>
-  <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A3">
-      <formula1>""</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B3">
-      <formula1>""</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C3">
-      <formula1>""</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3">
-      <formula1>""</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E3">
-      <formula1>""</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>